<commit_message>
Unesen effort za danas
</commit_message>
<xml_diff>
--- a/Effort_Evidence_Ime_Prezime.xlsx
+++ b/Effort_Evidence_Ime_Prezime.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Involved Engineers:</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>Trka automobila</t>
+  </si>
+  <si>
+    <t>Napisana nova funkcija za pomjeranje vozila.</t>
+  </si>
+  <si>
+    <t>Uslovi zadatka su promjenjeni na prijedlog tim lidera, broj vozila je sada 6 I za sada je izbacen uslov za preticanje.</t>
   </si>
   <si>
     <t>Kladionica</t>
@@ -276,7 +282,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -354,10 +360,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -417,7 +419,7 @@
   <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -479,7 +481,7 @@
       <c r="H3" s="18"/>
       <c r="I3" s="19"/>
       <c r="J3" s="19"/>
-      <c r="K3" s="20"/>
+      <c r="K3" s="18"/>
       <c r="L3" s="18"/>
       <c r="M3" s="18"/>
       <c r="N3" s="18"/>
@@ -488,398 +490,404 @@
       <c r="Q3" s="18"/>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="21" t="n">
+      <c r="A4" s="20" t="n">
         <v>42877</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="24"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="23"/>
       <c r="F4" s="16"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="21" t="n">
+      <c r="A5" s="20" t="n">
         <v>42878</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="24"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="23"/>
       <c r="F5" s="16"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="27" t="s">
+      <c r="G5" s="24"/>
+      <c r="H5" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="27" t="s">
+      <c r="I5" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="27" t="s">
+      <c r="J5" s="26" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="21" t="n">
+      <c r="A6" s="20" t="n">
         <v>42879</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="24"/>
+      <c r="E6" s="23"/>
       <c r="F6" s="16"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27" t="s">
+      <c r="G6" s="24"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="27" t="s">
+      <c r="J6" s="26" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="21" t="n">
+      <c r="A7" s="20" t="n">
         <v>42880</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="24"/>
+      <c r="B7" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="23"/>
       <c r="F7" s="16"/>
-      <c r="G7" s="25"/>
-      <c r="I7" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="27" t="s">
-        <v>15</v>
+      <c r="G7" s="24"/>
+      <c r="I7" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="26" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="21" t="n">
+      <c r="A8" s="20" t="n">
         <v>42881</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="24"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="23"/>
       <c r="F8" s="16"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="21" t="n">
+      <c r="A9" s="20" t="n">
         <v>42882</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="24"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="23"/>
       <c r="F9" s="16"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="21" t="n">
+      <c r="A10" s="20" t="n">
         <v>42883</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="24"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="23"/>
       <c r="F10" s="16"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="21" t="n">
+      <c r="A11" s="20" t="n">
         <v>42884</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="24"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="23"/>
       <c r="F11" s="16"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="21" t="n">
+      <c r="A12" s="20" t="n">
         <v>42885</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="24"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="23"/>
       <c r="F12" s="16"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="21" t="n">
+      <c r="A13" s="20" t="n">
         <v>42886</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="24"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="23"/>
       <c r="F13" s="16"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="21" t="n">
+      <c r="A14" s="20" t="n">
         <v>42887</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="24"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="23"/>
       <c r="F14" s="16"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="21" t="n">
+      <c r="A15" s="20" t="n">
         <v>42888</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="24"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="23"/>
       <c r="F15" s="16"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="21" t="n">
+      <c r="A16" s="20" t="n">
         <v>42889</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="24"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="23"/>
       <c r="F16" s="16"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="21" t="n">
+      <c r="A17" s="20" t="n">
         <v>42890</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="23"/>
       <c r="F17" s="16"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="21" t="n">
+      <c r="A18" s="20" t="n">
         <v>42891</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="24"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="23"/>
       <c r="F18" s="16"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="21" t="n">
+      <c r="A19" s="20" t="n">
         <v>42892</v>
       </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="24"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="23"/>
       <c r="F19" s="16"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="21" t="n">
+      <c r="A20" s="20" t="n">
         <v>42893</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="24"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="23"/>
       <c r="F20" s="16"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="21" t="n">
+      <c r="A21" s="20" t="n">
         <v>42894</v>
       </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="24"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="23"/>
       <c r="F21" s="16"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="21" t="n">
+      <c r="A22" s="20" t="n">
         <v>42895</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="24"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="23"/>
       <c r="F22" s="16"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="21" t="n">
+      <c r="A23" s="20" t="n">
         <v>42896</v>
       </c>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="24"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="23"/>
       <c r="F23" s="16"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="21" t="n">
+      <c r="A24" s="20" t="n">
         <v>42897</v>
       </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="24"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="23"/>
       <c r="F24" s="16"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="21" t="n">
+      <c r="A25" s="20" t="n">
         <v>42898</v>
       </c>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="24"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="23"/>
       <c r="F25" s="16"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="21" t="n">
+      <c r="A26" s="20" t="n">
         <v>42899</v>
       </c>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="24"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="23"/>
       <c r="F26" s="16"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="21" t="n">
+      <c r="A27" s="20" t="n">
         <v>42900</v>
       </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="24"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="23"/>
       <c r="F27" s="16"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="21" t="n">
+      <c r="A28" s="20" t="n">
         <v>42901</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="24"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="23"/>
       <c r="F28" s="16"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="21" t="n">
+      <c r="A29" s="20" t="n">
         <v>42902</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="24"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="23"/>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
       <c r="H29" s="16"/>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="21" t="n">
+      <c r="A30" s="20" t="n">
         <v>42903</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="24"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="23"/>
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
       <c r="H30" s="16"/>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="21" t="n">
+      <c r="A31" s="20" t="n">
         <v>42904</v>
       </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="24"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="23"/>
       <c r="F31" s="16"/>
       <c r="G31" s="16"/>
       <c r="H31" s="16"/>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="21" t="n">
+      <c r="A32" s="20" t="n">
         <v>42905</v>
       </c>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="24"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="23"/>
       <c r="F32" s="16"/>
       <c r="G32" s="16"/>
       <c r="H32" s="16"/>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="21" t="n">
+      <c r="A33" s="20" t="n">
         <v>42906</v>
       </c>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="24"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="23"/>
       <c r="F33" s="16"/>
       <c r="G33" s="16"/>
       <c r="H33" s="16"/>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="21" t="n">
+      <c r="A34" s="20" t="n">
         <v>42907</v>
       </c>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="24"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="23"/>
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
       <c r="H34" s="16"/>

</xml_diff>